<commit_message>
JSON to CSV conversion.
Minor changes to Excel to JSON conversion
ReadMe updated
</commit_message>
<xml_diff>
--- a/Sample Input Files/3_ExcelToJSON.xlsx
+++ b/Sample Input Files/3_ExcelToJSON.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabique.mp\Documents\whoiam\code\whoiam-internal\B2C Localization Tool\test-files\ToJson\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabique.mp\Documents\whoiam\code\whoiam-internal\B2C Localization Tool\Sample Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575AB54-C99D-43D7-9995-99209AC0CCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2354E79-E73B-4D40-B0D5-B640AFC2687B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
   <si>
     <t>Resource</t>
   </si>
@@ -1156,9 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,14 +1245,16 @@
       <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
+      <c r="L2" s="1" t="str">
+        <f>_xlfn.CONCAT("(Modified) ",K2)</f>
+        <v>(Modified) ¿Está seguro de que quiere cancelar la introducción de los detalles?</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
+      <c r="N2" s="1" t="str">
+        <f>_xlfn.CONCAT("(Modified) ",M2)</f>
+        <v>(Modified) ht-Are you sure that you want to cancel entering your details?</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1273,20 +1275,22 @@
         <v>14</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J29" si="0">_xlfn.CONCAT("(Modified) ",I3)</f>
+        <f t="shared" ref="J3:J30" si="0">_xlfn.CONCAT("(Modified) ",I3)</f>
         <v>(Modified) No</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>14</v>
+      <c r="L3" s="1" t="str">
+        <f t="shared" ref="L3:L30" si="1">_xlfn.CONCAT("(Modified) ",K3)</f>
+        <v>(Modified) No</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>15</v>
+      <c r="N3" s="1" t="str">
+        <f t="shared" ref="N3:N30" si="2">_xlfn.CONCAT("(Modified) ",M3)</f>
+        <v>(Modified) ht-No</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1313,14 +1317,16 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Cancelar la introducción de los detalles</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>19</v>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Cancel Entering Your Details</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1347,14 +1353,16 @@
       <c r="K5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>22</v>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Sí</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>23</v>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Yes</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1381,14 +1389,16 @@
       <c r="K6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>26</v>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Cancelar</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>27</v>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Cancel</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1415,14 +1425,16 @@
       <c r="K7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>30</v>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Continuar</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Continue</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1445,17 +1457,23 @@
       <c r="I8" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Your password must have at least {0} of the following:</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>36</v>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) La contraseña debe tener al menos {0} de los siguientes elementos:</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>37</v>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Your password must have at least {0} of the following:</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1478,17 +1496,23 @@
       <c r="I9" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Your password must have at least {0} of the following:</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>36</v>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) La contraseña debe tener al menos {0} de los siguientes elementos:</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>37</v>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Your password must have at least {0} of the following:</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1508,17 +1532,23 @@
       <c r="I10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Are you sure that you want to cancel entering your details?</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) ¿Está seguro de que quiere cancelar la introducción de los detalles?</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>12</v>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Are you sure that you want to cancel entering your details?</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1538,17 +1568,23 @@
       <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) No</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>14</v>
+      <c r="L11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) No</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>15</v>
+      <c r="N11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-No</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1568,17 +1604,23 @@
       <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Cancel Entering Your Details</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>18</v>
+      <c r="L12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Cancelar la introducción de los detalles</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>19</v>
+      <c r="N12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Cancel Entering Your Details</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1598,17 +1640,23 @@
       <c r="I13" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Yes</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>22</v>
+      <c r="L13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Sí</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>23</v>
+      <c r="N13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Yes</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1628,17 +1676,23 @@
       <c r="I14" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Cancel</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>26</v>
+      <c r="L14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Cancelar</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>27</v>
+      <c r="N14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Cancel</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1658,17 +1712,23 @@
       <c r="I15" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Continue</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>30</v>
+      <c r="L15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) Continuar</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>31</v>
+      <c r="N15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-Continue</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1688,17 +1748,23 @@
       <c r="I16" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) The user has cancelled entering self-asserted information</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>51</v>
+      <c r="L16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) El usuario ha cancelado la introducción de información afirmada por él mismo</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>52</v>
+      <c r="N16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-The user has cancelled entering self-asserted information</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1717,21 +1783,25 @@
       <c r="I17" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Sign up now</v>
+      </c>
       <c r="K17" s="1" t="str">
-        <f t="shared" ref="K17:L27" si="1">_xlfn.CONCAT("(es) ",I17)</f>
+        <f t="shared" ref="K17:L27" si="3">_xlfn.CONCAT("(es) ",I17)</f>
         <v>(es) Sign up now</v>
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Sign up now</v>
       </c>
       <c r="M17" s="1" t="str">
-        <f t="shared" ref="M17:N23" si="2">_xlfn.CONCAT("(ht)",I17)</f>
+        <f t="shared" ref="M17:N23" si="4">_xlfn.CONCAT("(ht)",I17)</f>
         <v>(ht)Sign up now</v>
       </c>
       <c r="N17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Sign up now</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1750,21 +1820,25 @@
       <c r="I18" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Sign up with {0} or {1}</v>
+      </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Sign up with {0} or {1}</v>
       </c>
       <c r="L18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Sign up with {0} or {1}</v>
       </c>
       <c r="M18" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Sign up with {0} or {1}</v>
       </c>
       <c r="N18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Sign up with {0} or {1}</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1783,21 +1857,25 @@
       <c r="I19" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Please enter your {0}</v>
+      </c>
       <c r="K19" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Please enter your {0}</v>
       </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Please enter your {0}</v>
       </c>
       <c r="M19" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Please enter your {0}</v>
       </c>
       <c r="N19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Please enter your {0}</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1816,21 +1894,25 @@
       <c r="I20" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="J20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Please enter a valid {0}</v>
+      </c>
       <c r="K20" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Please enter a valid {0}</v>
       </c>
       <c r="L20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Please enter a valid {0}</v>
       </c>
       <c r="M20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Please enter a valid {0}</v>
       </c>
       <c r="N20" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Please enter a valid {0}</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,21 +1931,25 @@
       <c r="I21" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Sign in</v>
+      </c>
       <c r="K21" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Sign in</v>
       </c>
       <c r="L21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Sign in</v>
       </c>
       <c r="M21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Sign in</v>
       </c>
       <c r="N21" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Sign in</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1882,21 +1968,25 @@
       <c r="I22" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Sign in with your {0}</v>
+      </c>
       <c r="K22" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Sign in with your {0}</v>
       </c>
       <c r="L22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Sign in with your {0}</v>
       </c>
       <c r="M22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Sign in with your {0}</v>
       </c>
       <c r="N22" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Sign in with your {0}</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,21 +2005,25 @@
       <c r="I23" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Sign up with {0}, {1}, or {2}</v>
+      </c>
       <c r="K23" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Sign up with {0}, {1}, or {2}</v>
       </c>
       <c r="L23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+        <v>(Modified) (es) Sign up with {0}, {1}, or {2}</v>
       </c>
       <c r="M23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>(ht)Sign up with {0}, {1}, or {2}</v>
       </c>
       <c r="N23" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>(ht)</v>
+        <v>(Modified) (ht)Sign up with {0}, {1}, or {2}</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1954,21 +2048,25 @@
       <c r="I24" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) New Password</v>
+      </c>
       <c r="K24" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) New Password</v>
       </c>
-      <c r="L24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+      <c r="L24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) (es) New Password</v>
       </c>
       <c r="M24" s="4" t="str">
-        <f t="shared" ref="M24:N27" si="3">_xlfn.CONCAT("(ht) ",I24)</f>
+        <f t="shared" ref="M24:N27" si="5">_xlfn.CONCAT("(ht) ",I24)</f>
         <v>(ht) New Password</v>
       </c>
-      <c r="N24" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">(ht) </v>
+      <c r="N24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) (ht) New Password</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1993,21 +2091,25 @@
       <c r="I25" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Enter new password</v>
+      </c>
       <c r="K25" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Enter new password</v>
       </c>
-      <c r="L25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+      <c r="L25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) (es) Enter new password</v>
       </c>
       <c r="M25" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(ht) Enter new password</v>
       </c>
-      <c r="N25" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">(ht) </v>
+      <c r="N25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) (ht) Enter new password</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2032,21 +2134,25 @@
       <c r="I26" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Confirm New Password</v>
+      </c>
       <c r="K26" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Confirm New Password</v>
       </c>
-      <c r="L26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+      <c r="L26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) (es) Confirm New Password</v>
       </c>
       <c r="M26" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(ht) Confirm New Password</v>
       </c>
-      <c r="N26" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">(ht) </v>
+      <c r="N26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) (ht) Confirm New Password</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2071,21 +2177,25 @@
       <c r="I27" s="5" t="s">
         <v>58</v>
       </c>
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Confirm new password</v>
+      </c>
       <c r="K27" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>(es) Confirm new password</v>
       </c>
-      <c r="L27" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">(es) </v>
+      <c r="L27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) (es) Confirm new password</v>
       </c>
       <c r="M27" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(ht) Confirm new password</v>
       </c>
-      <c r="N27" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">(ht) </v>
+      <c r="N27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) (ht) Confirm new password</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2108,17 +2218,23 @@
       <c r="I28" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) 8-16 characters, containing 3 out of 4 of the following: Lowercase characters, uppercase characters, digits (0-9), and one or more of the following symbols: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
+      </c>
       <c r="K28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>47</v>
+      <c r="L28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) 8 a 16 caracteres, que contengan 3 de los 4 tipos siguientes: caracteres en minúsculas, caracteres en mayúsculas, dígitos (0-9) y uno o más de los siguientes símbolos: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>46</v>
+      <c r="N28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-8-16 characters, containing 3 out of 4 of the following: Lowercase characters, uppercase characters, digits (0-9), and one or more of the following symbols: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2141,17 +2257,23 @@
       <c r="I29" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) 8-16 characters, containing 3 out of 4 of the following: Lowercase characters, uppercase characters, digits (0-9), and one or more of the following symbols: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
+      </c>
       <c r="K29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>47</v>
+      <c r="L29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) 8 a 16 caracteres, que contengan 3 de los 4 tipos siguientes: caracteres en minúsculas, caracteres en mayúsculas, dígitos (0-9) y uno o más de los siguientes símbolos: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>46</v>
+      <c r="N29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) ht-8-16 characters, containing 3 out of 4 of the following: Lowercase characters, uppercase characters, digits (0-9), and one or more of the following symbols: @ # $ % ^ &amp; * - _ + = [ ] { } | \ : ' , ? / ` ~ " ( ) ; .</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2176,18 +2298,23 @@
       <c r="I30" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(Modified) Enter the verification code</v>
+      </c>
       <c r="K30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L30" s="4" t="s">
-        <v>79</v>
+      <c r="L30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(Modified) (es) Enter the verification code</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N30" s="4" t="s">
-        <v>80</v>
+      <c r="N30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>(Modified) (ht) Enter the verification code</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>